<commit_message>
Update README.xlsx for BASIN_Stats_EFLOWSChg20_CurrrentStatePCT.xlsx spreadsheet
</commit_message>
<xml_diff>
--- a/README.xlsx
+++ b/README.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pamelagreen/Desktop/Data/Griffith2022/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8DBABF-5A03-5A45-8D4C-A9A80E2CC068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCD7733-9B3E-EF49-A642-AFCB0AF3BCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37400" yWindow="640" windowWidth="30360" windowHeight="17440" xr2:uid="{AC79CE72-321E-844F-A989-0FF187B9C603}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
   <si>
     <r>
       <rPr>
@@ -361,20 +361,26 @@
     <t>Proportion of months in a year with more than 20% difference between Pristine and Disturbed flow</t>
   </si>
   <si>
-    <t>Basin-level estimates of the proportion of grid cells where discharge is more than 20% different between Prostine and Disturbed flows</t>
-  </si>
-  <si>
     <t>Proportion of months in year</t>
   </si>
   <si>
     <t>Mutliple - see spreadsheet for units</t>
+  </si>
+  <si>
+    <t>BASIN_Stats_EFLOWSChg20_CurrrentStatePCT.xlsx</t>
+  </si>
+  <si>
+    <t>Basin-level data and Global calculations for total area and popultion inside Safe and Just Earth System limits for Surface Water (N2,N3)</t>
+  </si>
+  <si>
+    <t>Basin-level data and estimates of the proportion of grid cells where discharge is more than 20% different between Prostine and Disturbed flows</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -415,6 +421,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -436,13 +449,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1082,7 +1096,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998D523C-B220-F44C-B515-B79245E7605B}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -1090,10 +1104,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="114.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="122.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
@@ -1118,7 +1132,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
         <v>66</v>
@@ -1132,7 +1146,7 @@
         <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
         <v>66</v>
@@ -1146,10 +1160,24 @@
         <v>64</v>
       </c>
       <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
-        <v>67</v>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit README.xlsx to correct folder names
</commit_message>
<xml_diff>
--- a/README.xlsx
+++ b/README.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pamelagreen/Desktop/Data/Griffith2022/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCD7733-9B3E-EF49-A642-AFCB0AF3BCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22B2137-A888-7F4A-8FA7-2CCA303E7979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37400" yWindow="640" windowWidth="30360" windowHeight="17440" xr2:uid="{AC79CE72-321E-844F-A989-0FF187B9C603}"/>
   </bookViews>
@@ -150,16 +150,196 @@
     <t>Tabs:</t>
   </si>
   <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>GeoTiff</t>
+  </si>
+  <si>
+    <t>cellarea</t>
+  </si>
+  <si>
+    <t>population</t>
+  </si>
+  <si>
+    <t>RiverBasin</t>
+  </si>
+  <si>
+    <t>HydroSTN06_BasinMouth.shp</t>
+  </si>
+  <si>
+    <t>HydroSTN30_Confluence_6m.shp</t>
+  </si>
+  <si>
+    <t>Global_Basin_HydroSTN30_06min_GHAAS3.tif</t>
+  </si>
+  <si>
+    <t>HydroSTN06_Subbasin.tif</t>
+  </si>
+  <si>
+    <t>MajorBasinLookUp.xlsx</t>
+  </si>
+  <si>
+    <t>WBM_data</t>
+  </si>
+  <si>
+    <t>flow_mask.tif</t>
+  </si>
+  <si>
+    <t>WBM_TerraClimate_OUTPUTQ_PRIST_aLTM_2000-2020.tif</t>
+  </si>
+  <si>
+    <t>WBM_TerraClimate_OUTPUTQ_PRIST_mLTM_2000-2020.tif</t>
+  </si>
+  <si>
+    <t>WBM_TerraClimate_OUTPUTQ_DIST_aLTM_2000-2020.tif</t>
+  </si>
+  <si>
+    <t>WBM_TerraClimate_OUTPUTQ_DIST_mLTM_2000-2020.tif</t>
+  </si>
+  <si>
+    <t>WBM_TerraClimate_OUTPUT_IrrNetWD_mm_aLTM_2000-2020.tif</t>
+  </si>
+  <si>
+    <t>CellArea_6m.tif</t>
+  </si>
+  <si>
+    <t>Global_UpstreamAreakm2_6min.tif</t>
+  </si>
+  <si>
+    <t>gpw_v4_population_count_rev11_2020_6min.tif</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>km2</t>
+  </si>
+  <si>
+    <t>Basin IDs</t>
+  </si>
+  <si>
+    <t>Subbasin IDs</t>
+  </si>
+  <si>
+    <t>Subbasin Confluence Point file - IDs match Subbasin tif</t>
+  </si>
+  <si>
+    <t>Basin mouth Point file - IDs match Basin tiff</t>
+  </si>
+  <si>
+    <t>Basin names by Basin IDs</t>
+  </si>
+  <si>
+    <t>Downstream population counts (# people)</t>
+  </si>
+  <si>
+    <t>Binary (1=actively flowing, 0=non-flowing)</t>
+  </si>
+  <si>
+    <t>km3/yr</t>
+  </si>
+  <si>
+    <t>Gridded cellarea at 6-minute resolution</t>
+  </si>
+  <si>
+    <t>Uostream area from any point in river network</t>
+  </si>
+  <si>
+    <t>Discharge weighted downstream population</t>
+  </si>
+  <si>
+    <t>RGIS river basin extents</t>
+  </si>
+  <si>
+    <t>RGIS subbasin basin extents</t>
+  </si>
+  <si>
+    <t>RGIS river basin discharge point at mouth</t>
+  </si>
+  <si>
+    <t>RGIS subbasin discharge point at river confluence</t>
+  </si>
+  <si>
+    <t>Look up table for known Basin names</t>
+  </si>
+  <si>
+    <t>Annual long term Disturbed discharge from 2000-2020</t>
+  </si>
+  <si>
+    <t>Monthly long term Disturbed discharge from 2000-2020</t>
+  </si>
+  <si>
+    <t>Monthly long term Pristine discharge from 2000-2020</t>
+  </si>
+  <si>
+    <t>Annual long term Pristine discharge from 2000-2020</t>
+  </si>
+  <si>
+    <t>Mask for actively flowing river/stream extents</t>
+  </si>
+  <si>
+    <t>WBM modelled irrigation depths</t>
+  </si>
+  <si>
+    <t>mm/yr</t>
+  </si>
+  <si>
+    <t>Estress_WBM_TerraClimate_2000-2020_LTM_Chg20.tif</t>
+  </si>
+  <si>
+    <t>SUBBASIN_Stats_EFLOWSChg20.xlsx</t>
+  </si>
+  <si>
+    <t>BASIN_Stats_EFLOWSChg20.xlsx</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Shapefile</t>
+  </si>
+  <si>
+    <t>MSExcel</t>
+  </si>
+  <si>
+    <t>Output File</t>
+  </si>
+  <si>
+    <t>Proportion of months in a year with more than 20% difference between Pristine and Disturbed flow</t>
+  </si>
+  <si>
+    <t>Proportion of months in year</t>
+  </si>
+  <si>
+    <t>Mutliple - see spreadsheet for units</t>
+  </si>
+  <si>
+    <t>BASIN_Stats_EFLOWSChg20_CurrrentStatePCT.xlsx</t>
+  </si>
+  <si>
+    <t>Basin-level data and Global calculations for total area and popultion inside Safe and Just Earth System limits for Surface Water (N2,N3)</t>
+  </si>
+  <si>
+    <t>Basin-level data and estimates of the proportion of grid cells where discharge is more than 20% different between Prostine and Disturbed flows</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Input_files</t>
+      <t>ModelOutput</t>
     </r>
     <r>
       <rPr>
@@ -169,20 +349,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: lists all files contained in the directory 'ModelInput'. </t>
+      <t xml:space="preserve">: lists model output files contained in the folder 'ModelOutput'. </t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Output_files</t>
+      <t>ModelInput</t>
     </r>
     <r>
       <rPr>
@@ -192,195 +372,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: lists model output files contained in the directory 'ModelOutput'. </t>
+      <t xml:space="preserve">: lists  model input files contained in the folder 'ModelInput'. </t>
     </r>
-  </si>
-  <si>
-    <t>Folder</t>
-  </si>
-  <si>
-    <t>GeoTiff</t>
-  </si>
-  <si>
-    <t>cellarea</t>
-  </si>
-  <si>
-    <t>population</t>
-  </si>
-  <si>
-    <t>RiverBasin</t>
-  </si>
-  <si>
-    <t>HydroSTN06_BasinMouth.shp</t>
-  </si>
-  <si>
-    <t>HydroSTN30_Confluence_6m.shp</t>
-  </si>
-  <si>
-    <t>Global_Basin_HydroSTN30_06min_GHAAS3.tif</t>
-  </si>
-  <si>
-    <t>HydroSTN06_Subbasin.tif</t>
-  </si>
-  <si>
-    <t>MajorBasinLookUp.xlsx</t>
-  </si>
-  <si>
-    <t>WBM_data</t>
-  </si>
-  <si>
-    <t>flow_mask.tif</t>
-  </si>
-  <si>
-    <t>WBM_TerraClimate_OUTPUTQ_PRIST_aLTM_2000-2020.tif</t>
-  </si>
-  <si>
-    <t>WBM_TerraClimate_OUTPUTQ_PRIST_mLTM_2000-2020.tif</t>
-  </si>
-  <si>
-    <t>WBM_TerraClimate_OUTPUTQ_DIST_aLTM_2000-2020.tif</t>
-  </si>
-  <si>
-    <t>WBM_TerraClimate_OUTPUTQ_DIST_mLTM_2000-2020.tif</t>
-  </si>
-  <si>
-    <t>WBM_TerraClimate_OUTPUT_IrrNetWD_mm_aLTM_2000-2020.tif</t>
-  </si>
-  <si>
-    <t>CellArea_6m.tif</t>
-  </si>
-  <si>
-    <t>Global_UpstreamAreakm2_6min.tif</t>
-  </si>
-  <si>
-    <t>gpw_v4_population_count_rev11_2020_6min.tif</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>km2</t>
-  </si>
-  <si>
-    <t>Basin IDs</t>
-  </si>
-  <si>
-    <t>Subbasin IDs</t>
-  </si>
-  <si>
-    <t>Subbasin Confluence Point file - IDs match Subbasin tif</t>
-  </si>
-  <si>
-    <t>Basin mouth Point file - IDs match Basin tiff</t>
-  </si>
-  <si>
-    <t>Basin names by Basin IDs</t>
-  </si>
-  <si>
-    <t>Downstream population counts (# people)</t>
-  </si>
-  <si>
-    <t>Binary (1=actively flowing, 0=non-flowing)</t>
-  </si>
-  <si>
-    <t>km3/yr</t>
-  </si>
-  <si>
-    <t>Gridded cellarea at 6-minute resolution</t>
-  </si>
-  <si>
-    <t>Uostream area from any point in river network</t>
-  </si>
-  <si>
-    <t>Discharge weighted downstream population</t>
-  </si>
-  <si>
-    <t>RGIS river basin extents</t>
-  </si>
-  <si>
-    <t>RGIS subbasin basin extents</t>
-  </si>
-  <si>
-    <t>RGIS river basin discharge point at mouth</t>
-  </si>
-  <si>
-    <t>RGIS subbasin discharge point at river confluence</t>
-  </si>
-  <si>
-    <t>Look up table for known Basin names</t>
-  </si>
-  <si>
-    <t>Annual long term Disturbed discharge from 2000-2020</t>
-  </si>
-  <si>
-    <t>Monthly long term Disturbed discharge from 2000-2020</t>
-  </si>
-  <si>
-    <t>Monthly long term Pristine discharge from 2000-2020</t>
-  </si>
-  <si>
-    <t>Annual long term Pristine discharge from 2000-2020</t>
-  </si>
-  <si>
-    <t>Mask for actively flowing river/stream extents</t>
-  </si>
-  <si>
-    <t>WBM modelled irrigation depths</t>
-  </si>
-  <si>
-    <t>mm/yr</t>
-  </si>
-  <si>
-    <t>Estress_WBM_TerraClimate_2000-2020_LTM_Chg20.tif</t>
-  </si>
-  <si>
-    <t>SUBBASIN_Stats_EFLOWSChg20.xlsx</t>
-  </si>
-  <si>
-    <t>BASIN_Stats_EFLOWSChg20.xlsx</t>
-  </si>
-  <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Shapefile</t>
-  </si>
-  <si>
-    <t>MSExcel</t>
-  </si>
-  <si>
-    <t>Output File</t>
-  </si>
-  <si>
-    <t>Proportion of months in a year with more than 20% difference between Pristine and Disturbed flow</t>
-  </si>
-  <si>
-    <t>Proportion of months in year</t>
-  </si>
-  <si>
-    <t>Mutliple - see spreadsheet for units</t>
-  </si>
-  <si>
-    <t>BASIN_Stats_EFLOWSChg20_CurrrentStatePCT.xlsx</t>
-  </si>
-  <si>
-    <t>Basin-level data and Global calculations for total area and popultion inside Safe and Just Earth System limits for Surface Water (N2,N3)</t>
-  </si>
-  <si>
-    <t>Basin-level data and estimates of the proportion of grid cells where discharge is more than 20% different between Prostine and Disturbed flows</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -424,6 +424,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -773,9 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7BDF3D2-F8D8-2E4A-8090-DA540BF4D3A7}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -834,12 +840,12 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -866,227 +872,227 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1112,72 +1118,72 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
         <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
         <v>68</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>